<commit_message>
EEPROM neu (Makefile) eeprombyteschreiben zu EEPROM.write, dto mit ..lesen
</commit_message>
<xml_diff>
--- a/sendbuffer.xlsx
+++ b/sendbuffer.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/RC/RC_22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDA3D20E-77B9-AD42-8DA9-D08E8A395E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4E9102B-EF48-0644-98EF-12180BF557E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="2300" windowWidth="27840" windowHeight="16940" xr2:uid="{7FCFCFB2-E853-8C47-8EAB-18CEC4EE5340}"/>
+    <workbookView xWindow="13940" yWindow="3560" windowWidth="27840" windowHeight="16940" xr2:uid="{7FCFCFB2-E853-8C47-8EAB-18CEC4EE5340}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,10 +28,46 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>pot1L</t>
+  </si>
+  <si>
+    <t>pot0L</t>
+  </si>
+  <si>
+    <t>pot0H</t>
+  </si>
+  <si>
+    <t>pot1H</t>
+  </si>
+  <si>
+    <t>pot2L</t>
+  </si>
+  <si>
+    <t>pot2H</t>
+  </si>
+  <si>
+    <t>pot3L</t>
+  </si>
+  <si>
+    <t>pot3H</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52,7 +89,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,12 +97,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -380,12 +427,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B8F52AC-FBC5-C14E-BE36-C545DD4ADBAF}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>